<commit_message>
modified data (because there were some logic problems)& added python requirements & modified repport
</commit_message>
<xml_diff>
--- a/data-folder/Données_groupe_01.xlsx
+++ b/data-folder/Données_groupe_01.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jean\MIASHS\Projet\Fichiers_2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jean\MIASHS\Projet\Fichiers_2025new\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18570" windowHeight="8505"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="13200"/>
   </bookViews>
   <sheets>
     <sheet name="données01" sheetId="2" r:id="rId1"/>
@@ -467,24 +467,24 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>50.3</v>
+        <v>32.32</v>
       </c>
       <c r="B13">
         <v>37</v>
       </c>
       <c r="C13">
-        <v>84</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>46.88</v>
+        <v>8.91</v>
       </c>
       <c r="B14">
         <v>76</v>
       </c>
       <c r="C14">
-        <v>122</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -500,233 +500,233 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>22.45</v>
+        <v>16.72</v>
       </c>
       <c r="B16">
         <v>34</v>
       </c>
       <c r="C16">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>60.6</v>
+        <v>23.59</v>
       </c>
       <c r="B17">
         <v>58</v>
       </c>
       <c r="C17">
-        <v>113</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>26.8</v>
+        <v>22.759999999999998</v>
       </c>
       <c r="B18">
         <v>18</v>
       </c>
       <c r="C18">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>7.6899999999999995</v>
+        <v>5.96</v>
       </c>
       <c r="B19">
         <v>38</v>
       </c>
       <c r="C19">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>29.28</v>
+        <v>28.23</v>
       </c>
       <c r="B20">
         <v>11</v>
       </c>
       <c r="C20">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>36.65</v>
+        <v>8.129999999999999</v>
       </c>
       <c r="B21">
         <v>74</v>
       </c>
       <c r="C21">
-        <v>111</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>73.27</v>
+        <v>23.9</v>
       </c>
       <c r="B22">
         <v>62</v>
       </c>
       <c r="C22">
-        <v>127</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>31.669999999999998</v>
+        <v>6.6199999999999992</v>
       </c>
       <c r="B23">
         <v>77</v>
       </c>
       <c r="C23">
-        <v>110</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>72.989999999999995</v>
+        <v>43.87</v>
       </c>
       <c r="B24">
         <v>37</v>
       </c>
       <c r="C24">
-        <v>102</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>37.619999999999997</v>
+        <v>33.31</v>
       </c>
       <c r="B25">
         <v>18</v>
       </c>
       <c r="C25">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>66.069999999999993</v>
+        <v>41.47</v>
       </c>
       <c r="B26">
         <v>35</v>
       </c>
       <c r="C26">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>33.56</v>
+        <v>9.19</v>
       </c>
       <c r="B27">
         <v>72</v>
       </c>
       <c r="C27">
-        <v>106</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>25.81</v>
+        <v>9.0399999999999991</v>
       </c>
       <c r="B28">
         <v>72</v>
       </c>
       <c r="C28">
-        <v>97</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>14.56</v>
+        <v>3.17</v>
       </c>
       <c r="B29">
         <v>85</v>
       </c>
       <c r="C29">
-        <v>100</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>62.480000000000004</v>
+        <v>38.279999999999994</v>
       </c>
       <c r="B30">
         <v>36</v>
       </c>
       <c r="C30">
-        <v>94</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>97.67</v>
+        <v>83.71</v>
       </c>
       <c r="B31">
         <v>17</v>
       </c>
       <c r="C31">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>69.27</v>
+        <v>34</v>
       </c>
       <c r="B32">
         <v>46</v>
       </c>
       <c r="C32">
-        <v>109</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>3.94</v>
+        <v>3.1</v>
       </c>
       <c r="B33">
         <v>33</v>
       </c>
       <c r="C33">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>79.38</v>
+        <v>26.35</v>
       </c>
       <c r="B34">
         <v>61</v>
       </c>
       <c r="C34">
-        <v>130</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>88.33</v>
+        <v>4.1099999999999994</v>
       </c>
       <c r="B35">
         <v>87</v>
       </c>
       <c r="C35">
-        <v>164</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>84.23</v>
+        <v>20.91</v>
       </c>
       <c r="B36">
         <v>67</v>
       </c>
       <c r="C36">
-        <v>141</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -742,35 +742,35 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>80.289999999999992</v>
+        <v>6.1400000000000006</v>
       </c>
       <c r="B38">
         <v>84</v>
       </c>
       <c r="C38">
-        <v>156</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>50.12</v>
+        <v>20.599999999999998</v>
       </c>
       <c r="B39">
         <v>55</v>
       </c>
       <c r="C39">
-        <v>104</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>47.06</v>
+        <v>30.270000000000003</v>
       </c>
       <c r="B40">
         <v>35</v>
       </c>
       <c r="C40">
-        <v>81</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -786,46 +786,46 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>33.81</v>
+        <v>3.2</v>
       </c>
       <c r="B42">
         <v>87</v>
       </c>
       <c r="C42">
-        <v>122</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>94.62</v>
+        <v>29.659999999999997</v>
       </c>
       <c r="B43">
         <v>60</v>
       </c>
       <c r="C43">
-        <v>141</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>9.5500000000000007</v>
+        <v>4.3600000000000003</v>
       </c>
       <c r="B44">
         <v>69</v>
       </c>
       <c r="C44">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>40.92</v>
+        <v>7.9</v>
       </c>
       <c r="B45">
         <v>76</v>
       </c>
       <c r="C45">
-        <v>117</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -841,24 +841,24 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>89.77000000000001</v>
+        <v>23.880000000000003</v>
       </c>
       <c r="B47">
         <v>66</v>
       </c>
       <c r="C47">
-        <v>143</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>8.51</v>
+        <v>2.48</v>
       </c>
       <c r="B48">
         <v>78</v>
       </c>
       <c r="C48">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -874,35 +874,35 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>59.489999999999995</v>
+        <v>17.34</v>
       </c>
       <c r="B50">
         <v>65</v>
       </c>
       <c r="C50">
-        <v>121</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>55.66</v>
+        <v>19.53</v>
       </c>
       <c r="B51">
         <v>61</v>
       </c>
       <c r="C51">
-        <v>113</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>20.7</v>
+        <v>9.5299999999999994</v>
       </c>
       <c r="B52">
         <v>56</v>
       </c>
       <c r="C52">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -918,90 +918,90 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>29.57</v>
+        <v>11.51</v>
       </c>
       <c r="B54">
         <v>68</v>
       </c>
       <c r="C54">
-        <v>96</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>24.98</v>
+        <v>4.9799999999999995</v>
       </c>
       <c r="B55">
         <v>87</v>
       </c>
       <c r="C55">
-        <v>111</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>41.949999999999996</v>
+        <v>23.98</v>
       </c>
       <c r="B56">
         <v>44</v>
       </c>
       <c r="C56">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>67.569999999999993</v>
+        <v>46.239999999999995</v>
       </c>
       <c r="B57">
         <v>31</v>
       </c>
       <c r="C57">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>69.47</v>
+        <v>44.26</v>
       </c>
       <c r="B58">
         <v>34</v>
       </c>
       <c r="C58">
-        <v>97</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>16.16</v>
+        <v>10.620000000000001</v>
       </c>
       <c r="B59">
         <v>37</v>
       </c>
       <c r="C59">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>39.14</v>
+        <v>24.279999999999998</v>
       </c>
       <c r="B60">
         <v>37</v>
       </c>
       <c r="C60">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>45.660000000000004</v>
+        <v>11.83</v>
       </c>
       <c r="B61">
         <v>71</v>
       </c>
       <c r="C61">
-        <v>115</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>